<commit_message>
Actualización de Burndown Chart
</commit_message>
<xml_diff>
--- a/Desarrollo/Edutec/Gestión/Sprint 1/Sprint Backlog - S1.xlsx
+++ b/Desarrollo/Edutec/Gestión/Sprint 1/Sprint Backlog - S1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspaces\Universidad\Edutec\Desarrollo\Edutec\Gestión\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D5860E-BDC8-4EBF-9484-CB7536BB3E93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FACFA34-CD05-4D59-B2D2-BC63D2A369DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1257,19 +1257,13 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1282,6 +1276,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1508,8 +1508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1005"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1842,17 +1842,17 @@
       <c r="Z10" s="3"/>
     </row>
     <row r="11" spans="1:26" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="118" t="s">
+      <c r="A11" s="127" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="119"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
-      <c r="G11" s="119"/>
-      <c r="H11" s="119"/>
-      <c r="I11" s="120"/>
+      <c r="B11" s="128"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="128"/>
+      <c r="F11" s="128"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="128"/>
+      <c r="I11" s="129"/>
       <c r="J11" s="3"/>
       <c r="K11" s="12"/>
       <c r="L11" s="3"/>
@@ -1888,7 +1888,7 @@
         <v>23</v>
       </c>
       <c r="F12" s="17">
-        <v>44508</v>
+        <v>44509</v>
       </c>
       <c r="G12" s="17">
         <v>44510</v>
@@ -3044,11 +3044,11 @@
       <c r="Z38" s="3"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="125" t="s">
+      <c r="A39" s="120" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="126"/>
-      <c r="C39" s="126"/>
+      <c r="B39" s="121"/>
+      <c r="C39" s="121"/>
       <c r="D39" s="122"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
@@ -3074,7 +3074,7 @@
       <c r="Z39" s="3"/>
     </row>
     <row r="40" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="121" t="s">
+      <c r="A40" s="130" t="s">
         <v>55</v>
       </c>
       <c r="B40" s="122"/>
@@ -3108,10 +3108,10 @@
       <c r="Z40" s="3"/>
     </row>
     <row r="41" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="123" t="s">
+      <c r="A41" s="118" t="s">
         <v>58</v>
       </c>
-      <c r="B41" s="124"/>
+      <c r="B41" s="119"/>
       <c r="C41" s="55" t="s">
         <v>19</v>
       </c>
@@ -3142,10 +3142,10 @@
       <c r="Z41" s="3"/>
     </row>
     <row r="42" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="123" t="s">
+      <c r="A42" s="118" t="s">
         <v>59</v>
       </c>
-      <c r="B42" s="124"/>
+      <c r="B42" s="119"/>
       <c r="C42" s="55" t="s">
         <v>35</v>
       </c>
@@ -3176,10 +3176,10 @@
       <c r="Z42" s="3"/>
     </row>
     <row r="43" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="123" t="s">
+      <c r="A43" s="118" t="s">
         <v>60</v>
       </c>
-      <c r="B43" s="124"/>
+      <c r="B43" s="119"/>
       <c r="C43" s="55" t="s">
         <v>41</v>
       </c>
@@ -3210,10 +3210,10 @@
       <c r="Z43" s="3"/>
     </row>
     <row r="44" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="123" t="s">
+      <c r="A44" s="118" t="s">
         <v>61</v>
       </c>
-      <c r="B44" s="124"/>
+      <c r="B44" s="119"/>
       <c r="C44" s="55" t="s">
         <v>47</v>
       </c>
@@ -3306,10 +3306,10 @@
       <c r="B47" s="82" t="s">
         <v>112</v>
       </c>
-      <c r="C47" s="127" t="s">
+      <c r="C47" s="123" t="s">
         <v>113</v>
       </c>
-      <c r="D47" s="127"/>
+      <c r="D47" s="123"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -3340,10 +3340,10 @@
       <c r="B48" s="84">
         <v>1</v>
       </c>
-      <c r="C48" s="128" t="s">
+      <c r="C48" s="124" t="s">
         <v>115</v>
       </c>
-      <c r="D48" s="129"/>
+      <c r="D48" s="125"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -3374,10 +3374,10 @@
       <c r="B49" s="84">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C49" s="130" t="s">
+      <c r="C49" s="126" t="s">
         <v>116</v>
       </c>
-      <c r="D49" s="129"/>
+      <c r="D49" s="125"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -30171,16 +30171,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A11:I11"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
     <mergeCell ref="A44:B44"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="C47:D47"/>
     <mergeCell ref="C48:D48"/>
     <mergeCell ref="C49:D49"/>
-    <mergeCell ref="A11:I11"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -31429,14 +31429,14 @@
       <c r="A11" s="132" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="119"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
-      <c r="F11" s="119"/>
-      <c r="G11" s="119"/>
-      <c r="H11" s="119"/>
-      <c r="I11" s="120"/>
+      <c r="B11" s="128"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="128"/>
+      <c r="F11" s="128"/>
+      <c r="G11" s="128"/>
+      <c r="H11" s="128"/>
+      <c r="I11" s="129"/>
       <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -31634,14 +31634,14 @@
       <c r="A18" s="132" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="119"/>
-      <c r="C18" s="119"/>
-      <c r="D18" s="119"/>
-      <c r="E18" s="119"/>
-      <c r="F18" s="119"/>
-      <c r="G18" s="119"/>
-      <c r="H18" s="119"/>
-      <c r="I18" s="120"/>
+      <c r="B18" s="128"/>
+      <c r="C18" s="128"/>
+      <c r="D18" s="128"/>
+      <c r="E18" s="128"/>
+      <c r="F18" s="128"/>
+      <c r="G18" s="128"/>
+      <c r="H18" s="128"/>
+      <c r="I18" s="129"/>
     </row>
     <row r="19" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="74" t="s">
@@ -31865,13 +31865,13 @@
         <v>54</v>
       </c>
       <c r="B28" s="134"/>
-      <c r="C28" s="124"/>
+      <c r="C28" s="119"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="135" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="124"/>
+      <c r="B29" s="119"/>
       <c r="C29" s="53" t="s">
         <v>56</v>
       </c>
@@ -31883,7 +31883,7 @@
       <c r="A30" s="131" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="124"/>
+      <c r="B30" s="119"/>
       <c r="C30" s="78" t="s">
         <v>35</v>
       </c>
@@ -31895,7 +31895,7 @@
       <c r="A31" s="131" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="124"/>
+      <c r="B31" s="119"/>
       <c r="C31" s="78" t="s">
         <v>63</v>
       </c>
@@ -31907,7 +31907,7 @@
       <c r="A32" s="131" t="s">
         <v>107</v>
       </c>
-      <c r="B32" s="124"/>
+      <c r="B32" s="119"/>
       <c r="C32" s="78" t="s">
         <v>73</v>
       </c>
@@ -31919,7 +31919,7 @@
       <c r="A33" s="131" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="124"/>
+      <c r="B33" s="119"/>
       <c r="C33" s="78" t="s">
         <v>69</v>
       </c>
@@ -31931,7 +31931,7 @@
       <c r="A34" s="131" t="s">
         <v>109</v>
       </c>
-      <c r="B34" s="124"/>
+      <c r="B34" s="119"/>
       <c r="C34" s="78" t="s">
         <v>71</v>
       </c>
@@ -31943,7 +31943,7 @@
       <c r="A35" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="B35" s="124"/>
+      <c r="B35" s="119"/>
       <c r="C35" s="78" t="s">
         <v>66</v>
       </c>

</xml_diff>